<commit_message>
testplanner: Change the default template
Signed-off-by: Jan Bylicki <jbylicki@antmicro.com>
</commit_message>
<xml_diff>
--- a/testplanner/testplan-tpl.xlsx
+++ b/testplanner/testplan-tpl.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ID:</t>
   </si>
@@ -28,6 +28,9 @@
     <t>Metric</t>
   </si>
   <si>
+    <t>Testbench</t>
+  </si>
+  <si>
     <t>Intent</t>
   </si>
   <si>
@@ -35,6 +38,9 @@
   </si>
   <si>
     <t>Checking Mechanism</t>
+  </si>
+  <si>
+    <t>Coverpoints</t>
   </si>
   <si>
     <t>Assignee</t>
@@ -344,7 +350,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="3.63"/>
     <col customWidth="1" min="2" max="2" width="25.38"/>
-    <col customWidth="1" min="12" max="12" width="11.0"/>
+    <col customWidth="1" min="14" max="14" width="11.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -399,8 +405,12 @@
       <c r="O2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="P2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -410,10 +420,12 @@
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B1:Q1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>